<commit_message>
constrain T > 3500 to remove M dwarfs; try to crossmatch with Ralf's results
</commit_message>
<xml_diff>
--- a/results/merged_result_MJ_with_properties.xlsx
+++ b/results/merged_result_MJ_with_properties.xlsx
@@ -1745,7 +1745,7 @@
       </c>
       <c r="AV7" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -2949,7 +2949,7 @@
       </c>
       <c r="AV14" t="inlineStr">
         <is>
-          <t>Brightest</t>
+          <t>Bright</t>
         </is>
       </c>
     </row>
@@ -5865,7 +5865,7 @@
       </c>
       <c r="AV31" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -7242,7 +7242,7 @@
       </c>
       <c r="AV39" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="AV49" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -10472,7 +10472,7 @@
       </c>
       <c r="AV58" t="inlineStr">
         <is>
-          <t>Dim</t>
+          <t>Dimmer</t>
         </is>
       </c>
     </row>
@@ -10642,7 +10642,7 @@
       </c>
       <c r="AV59" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -10815,7 +10815,7 @@
       </c>
       <c r="AV60" t="inlineStr">
         <is>
-          <t>Dim</t>
+          <t>Dimmer</t>
         </is>
       </c>
     </row>
@@ -14639,7 +14639,7 @@
       </c>
       <c r="AV83" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -15221,7 +15221,7 @@
       </c>
       <c r="AV87" t="inlineStr">
         <is>
-          <t>Dim</t>
+          <t>Dimmer</t>
         </is>
       </c>
     </row>
@@ -16582,7 +16582,7 @@
       </c>
       <c r="AV95" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>
@@ -17602,7 +17602,7 @@
       </c>
       <c r="AV101" t="inlineStr">
         <is>
-          <t>Dim</t>
+          <t>Dimmer</t>
         </is>
       </c>
     </row>
@@ -18107,7 +18107,7 @@
       </c>
       <c r="AV104" t="inlineStr">
         <is>
-          <t>Bright</t>
+          <t>Dim</t>
         </is>
       </c>
     </row>

</xml_diff>